<commit_message>
Changes on 25th May
</commit_message>
<xml_diff>
--- a/Practice Data/Math.xlsx
+++ b/Practice Data/Math.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shiva\OneDrive\Desktop\Shiva\UiPath Coaching\Batch 4\UiPathTraining_Batch4\Practice Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A913A54-8DCB-4926-B82E-ADC840F6CDDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B5DF5D-2BC7-4E4C-93E9-0FB745D90DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="4890" yWindow="350" windowWidth="14400" windowHeight="7270" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MathData" sheetId="2" r:id="rId1"/>
+    <sheet name="Math" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="8">
   <si>
     <t>Num1</t>
   </si>
@@ -55,8 +56,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -84,9 +93,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -371,8 +386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EABB8BED-E44D-4499-A44B-BBEABBC7CBD8}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D20"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -606,4 +621,124 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EDFA1B-30B3-4EF4-9BB4-DE536E3F19D2}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>5811</v>
+      </c>
+      <c r="B2" s="1">
+        <v>7944</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3">
+        <v>13755</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>330</v>
+      </c>
+      <c r="B3" s="1">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>883</v>
+      </c>
+      <c r="B4" s="1">
+        <v>7558</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>9098</v>
+      </c>
+      <c r="B5" s="1">
+        <v>7718</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1559</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>761</v>
+      </c>
+      <c r="B7" s="1">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>3911</v>
+      </c>
+      <c r="B8" s="1">
+        <v>93</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>